<commit_message>
changed operational gain loss to input in 24MS_MTOM_V1.0.202009.9006_MTOM
added excel comparison file for 24 MS run (dev vs official)
</commit_message>
<xml_diff>
--- a/RW Files/TestModelRuns/09_September Models/Sept24MS_OpVsDev_MOST.xlsx
+++ b/RW Files/TestModelRuns/09_September Models/Sept24MS_OpVsDev_MOST.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apivarnik\Desktop\GIT\MTOM\RW Files\TestModelRuns\09_September\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apivarnik\Desktop\GIT\MTOM\RW Files\TestModelRuns\09_September Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133C110C-8124-4651-8F34-8818C8DBF640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100A01A1-CDC4-4B4F-B2F4-2C26E0E6C083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="790" activeTab="8" xr2:uid="{ACA32295-86C6-4435-AED7-5BA48188675B}"/>
   </bookViews>
@@ -608,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -645,7 +645,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -2102,7 +2104,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17034,7 +17036,7 @@
   <dimension ref="A1:CI28"/>
   <sheetViews>
     <sheetView topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CG20" sqref="CG20"/>
+      <selection activeCell="CE21" sqref="CE21:CE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30241,11 +30243,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB02CDC5-0958-4E5D-9420-56BC4EECF463}">
   <dimension ref="A1:AU32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AU30"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
@@ -30568,7 +30618,7 @@
         <v>0.80510000000000004</v>
       </c>
       <c r="P3">
-        <v>256.199805840387</v>
+        <v>257.76048675959402</v>
       </c>
       <c r="Q3">
         <v>661273.58411413897</v>
@@ -30711,7 +30761,7 @@
         <v>0.74309999999999998</v>
       </c>
       <c r="P4">
-        <v>294.26472564397</v>
+        <v>295.73721775567498</v>
       </c>
       <c r="Q4">
         <v>745246.51009193598</v>
@@ -30854,7 +30904,7 @@
         <v>0.86799999999999999</v>
       </c>
       <c r="P5">
-        <v>266.52171801626503</v>
+        <v>268.09939425924802</v>
       </c>
       <c r="Q5">
         <v>687582.62385667395</v>
@@ -30997,7 +31047,7 @@
         <v>0.86819999999999997</v>
       </c>
       <c r="P6">
-        <v>170.302762939985</v>
+        <v>172.20749902874201</v>
       </c>
       <c r="Q6">
         <v>444467.13677680498</v>
@@ -31140,7 +31190,7 @@
         <v>0.80489999999999995</v>
       </c>
       <c r="P7">
-        <v>203.95775437887499</v>
+        <v>205.74528472295799</v>
       </c>
       <c r="Q7">
         <v>518562.77750649798</v>
@@ -31283,7 +31333,7 @@
         <v>0.67400000000000004</v>
       </c>
       <c r="P8">
-        <v>203.834410510586</v>
+        <v>205.307716184312</v>
       </c>
       <c r="Q8">
         <v>519289.44294144399</v>
@@ -31426,7 +31476,7 @@
         <v>0.69899999999999995</v>
       </c>
       <c r="P9">
-        <v>393.66804982203701</v>
+        <v>394.786562917634</v>
       </c>
       <c r="Q9">
         <v>968077.44428775099</v>
@@ -31569,7 +31619,7 @@
         <v>0.69889999999999997</v>
       </c>
       <c r="P10">
-        <v>417.491196597743</v>
+        <v>418.44576999364301</v>
       </c>
       <c r="Q10">
         <v>1032455.5454496701</v>
@@ -31712,7 +31762,7 @@
         <v>0.87709999999999999</v>
       </c>
       <c r="P11">
-        <v>386.16330465035202</v>
+        <v>387.51434734484098</v>
       </c>
       <c r="Q11">
         <v>993183.52537977602</v>
@@ -31855,7 +31905,7 @@
         <v>1</v>
       </c>
       <c r="P12">
-        <v>368.057847067659</v>
+        <v>369.47601529990402</v>
       </c>
       <c r="Q12">
         <v>947601.25495365204</v>
@@ -31998,7 +32048,7 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>321.13012875391701</v>
+        <v>322.72850677235499</v>
       </c>
       <c r="Q13">
         <v>827437.65215723298</v>
@@ -32141,7 +32191,7 @@
         <v>1</v>
       </c>
       <c r="P14">
-        <v>304.16779258256298</v>
+        <v>305.80707616952498</v>
       </c>
       <c r="Q14">
         <v>786453.41303552699</v>
@@ -32284,7 +32334,7 @@
         <v>1</v>
       </c>
       <c r="P15">
-        <v>274.53072256327698</v>
+        <v>276.16424462710802</v>
       </c>
       <c r="Q15">
         <v>713702.59411926998</v>
@@ -32427,7 +32477,7 @@
         <v>0.90990000000000004</v>
       </c>
       <c r="P16">
-        <v>203.18599623578001</v>
+        <v>205.024820856307</v>
       </c>
       <c r="Q16">
         <v>521072.70266180002</v>
@@ -32570,7 +32620,7 @@
         <v>0.58409999999999995</v>
       </c>
       <c r="P17">
-        <v>253.506600951173</v>
+        <v>254.849652019384</v>
       </c>
       <c r="Q17">
         <v>639724.71578436904</v>
@@ -32713,7 +32763,7 @@
         <v>0.80879999999999996</v>
       </c>
       <c r="P18">
-        <v>185.89001411759401</v>
+        <v>187.73014183404001</v>
       </c>
       <c r="Q18">
         <v>477115.46245457901</v>
@@ -32856,7 +32906,7 @@
         <v>0.8044</v>
       </c>
       <c r="P19">
-        <v>204.98737500215699</v>
+        <v>206.77400440067601</v>
       </c>
       <c r="Q19">
         <v>519512.82360885403</v>
@@ -32999,7 +33049,7 @@
         <v>0.67400000000000004</v>
       </c>
       <c r="P20">
-        <v>205.034666139965</v>
+        <v>206.50661886358901</v>
       </c>
       <c r="Q20">
         <v>520629.248100686</v>
@@ -33142,7 +33192,7 @@
         <v>0.69899999999999995</v>
       </c>
       <c r="P21">
-        <v>395.91819334569902</v>
+        <v>397.034793615019</v>
       </c>
       <c r="Q21">
         <v>970281.93146117497</v>
@@ -33285,7 +33335,7 @@
         <v>0.69889999999999997</v>
       </c>
       <c r="P22">
-        <v>419.933930739022</v>
+        <v>420.88661916362298</v>
       </c>
       <c r="Q22">
         <v>1034747.94482041</v>
@@ -33428,7 +33478,7 @@
         <v>0.87709999999999999</v>
       </c>
       <c r="P23">
-        <v>388.83563004779597</v>
+        <v>390.18454399897098</v>
       </c>
       <c r="Q23">
         <v>996078.71291693102</v>
@@ -33571,7 +33621,7 @@
         <v>1</v>
       </c>
       <c r="P24">
-        <v>370.56826182331298</v>
+        <v>371.98505127818902</v>
       </c>
       <c r="Q24">
         <v>950106.92943775305</v>
@@ -33714,7 +33764,7 @@
         <v>1</v>
       </c>
       <c r="P25">
-        <v>323.12117616554502</v>
+        <v>324.71855253392101</v>
       </c>
       <c r="Q25">
         <v>829372.31793929904</v>
@@ -33857,7 +33907,7 @@
         <v>1</v>
       </c>
       <c r="P26">
-        <v>305.89875166303</v>
+        <v>307.53720217549801</v>
       </c>
       <c r="Q26">
         <v>788103.07881759305</v>
@@ -34000,7 +34050,7 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <v>276.24651003498798</v>
+        <v>277.87872211873901</v>
       </c>
       <c r="Q27">
         <v>715701.34264297795</v>
@@ -34540,8 +34590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615FB051-7AE9-4A87-803F-04946A35F9AB}">
   <dimension ref="A1:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34561,7 +34611,7 @@
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -34606,7 +34656,7 @@
       <c r="O1" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="22" t="s">
         <v>133</v>
       </c>
       <c r="Q1" t="s">
@@ -34743,7 +34793,7 @@
       <c r="O2" t="s">
         <v>164</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="22" t="s">
         <v>116</v>
       </c>
       <c r="Q2" t="s">
@@ -34899,9 +34949,9 @@
         <f>Monthly_Op_LC!O3-Monthly_Dev_LC!O3</f>
         <v>0</v>
       </c>
-      <c r="P3" s="21">
+      <c r="P3" s="23">
         <f>Monthly_Op_LC!P3-Monthly_Dev_LC!P3</f>
-        <v>1.5606809196129916</v>
+        <v>4.0597569750389084E-10</v>
       </c>
       <c r="Q3" s="6">
         <f>Monthly_Op_LC!Q3-Monthly_Dev_LC!Q3</f>
@@ -35087,9 +35137,9 @@
         <f>Monthly_Op_LC!O4-Monthly_Dev_LC!O4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="23">
         <f>Monthly_Op_LC!P4-Monthly_Dev_LC!P4</f>
-        <v>1.472492112030011</v>
+        <v>3.2503066904610023E-10</v>
       </c>
       <c r="Q4" s="6">
         <f>Monthly_Op_LC!Q4-Monthly_Dev_LC!Q4</f>
@@ -35275,9 +35325,9 @@
         <f>Monthly_Op_LC!O5-Monthly_Dev_LC!O5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="23">
         <f>Monthly_Op_LC!P5-Monthly_Dev_LC!P5</f>
-        <v>1.5776762327349729</v>
+        <v>-1.0248015769320773E-8</v>
       </c>
       <c r="Q5" s="6">
         <f>Monthly_Op_LC!Q5-Monthly_Dev_LC!Q5</f>
@@ -35463,9 +35513,9 @@
         <f>Monthly_Op_LC!O6-Monthly_Dev_LC!O6</f>
         <v>0</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="23">
         <f>Monthly_Op_LC!P6-Monthly_Dev_LC!P6</f>
-        <v>1.9047360890149889</v>
+        <v>2.5798385649977718E-10</v>
       </c>
       <c r="Q6" s="6">
         <f>Monthly_Op_LC!Q6-Monthly_Dev_LC!Q6</f>
@@ -35651,9 +35701,9 @@
         <f>Monthly_Op_LC!O7-Monthly_Dev_LC!O7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="23">
         <f>Monthly_Op_LC!P7-Monthly_Dev_LC!P7</f>
-        <v>1.7875303421249953</v>
+        <v>-1.9579999843699625E-9</v>
       </c>
       <c r="Q7" s="6">
         <f>Monthly_Op_LC!Q7-Monthly_Dev_LC!Q7</f>
@@ -35836,9 +35886,9 @@
         <f>Monthly_Op_LC!O8-Monthly_Dev_LC!O8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="21">
+      <c r="P8" s="23">
         <f>Monthly_Op_LC!P8-Monthly_Dev_LC!P8</f>
-        <v>1.4733056744140072</v>
+        <v>6.8800432018178981E-10</v>
       </c>
       <c r="Q8" s="6">
         <f>Monthly_Op_LC!Q8-Monthly_Dev_LC!Q8</f>
@@ -36021,9 +36071,9 @@
         <f>Monthly_Op_LC!O9-Monthly_Dev_LC!O9</f>
         <v>0</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="23">
         <f>Monthly_Op_LC!P9-Monthly_Dev_LC!P9</f>
-        <v>1.1185130969629995</v>
+        <v>1.3660041986440774E-9</v>
       </c>
       <c r="Q9" s="6">
         <f>Monthly_Op_LC!Q9-Monthly_Dev_LC!Q9</f>
@@ -36206,9 +36256,9 @@
         <f>Monthly_Op_LC!O10-Monthly_Dev_LC!O10</f>
         <v>0</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="23">
         <f>Monthly_Op_LC!P10-Monthly_Dev_LC!P10</f>
-        <v>0.95457343825700036</v>
+        <v>4.2356987250968814E-8</v>
       </c>
       <c r="Q10" s="6">
         <f>Monthly_Op_LC!Q10-Monthly_Dev_LC!Q10</f>
@@ -36391,9 +36441,9 @@
         <f>Monthly_Op_LC!O11-Monthly_Dev_LC!O11</f>
         <v>0</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="23">
         <f>Monthly_Op_LC!P11-Monthly_Dev_LC!P11</f>
-        <v>1.3510426976479835</v>
+        <v>3.1590161597705446E-9</v>
       </c>
       <c r="Q11" s="6">
         <f>Monthly_Op_LC!Q11-Monthly_Dev_LC!Q11</f>
@@ -36576,9 +36626,9 @@
         <f>Monthly_Op_LC!O12-Monthly_Dev_LC!O12</f>
         <v>0</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="23">
         <f>Monthly_Op_LC!P12-Monthly_Dev_LC!P12</f>
-        <v>1.4181682063410221</v>
+        <v>-2.5904000722221099E-8</v>
       </c>
       <c r="Q12" s="6">
         <f>Monthly_Op_LC!Q12-Monthly_Dev_LC!Q12</f>
@@ -36761,9 +36811,9 @@
         <f>Monthly_Op_LC!O13-Monthly_Dev_LC!O13</f>
         <v>0</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="23">
         <f>Monthly_Op_LC!P13-Monthly_Dev_LC!P13</f>
-        <v>1.598378039083002</v>
+        <v>2.0645018139475724E-8</v>
       </c>
       <c r="Q13" s="6">
         <f>Monthly_Op_LC!Q13-Monthly_Dev_LC!Q13</f>
@@ -36946,9 +36996,9 @@
         <f>Monthly_Op_LC!O14-Monthly_Dev_LC!O14</f>
         <v>0</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="23">
         <f>Monthly_Op_LC!P14-Monthly_Dev_LC!P14</f>
-        <v>1.6392835884370243</v>
+        <v>1.4750298760191072E-9</v>
       </c>
       <c r="Q14" s="6">
         <f>Monthly_Op_LC!Q14-Monthly_Dev_LC!Q14</f>
@@ -37131,9 +37181,9 @@
         <f>Monthly_Op_LC!O15-Monthly_Dev_LC!O15</f>
         <v>0</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="23">
         <f>Monthly_Op_LC!P15-Monthly_Dev_LC!P15</f>
-        <v>1.6335220657230138</v>
+        <v>1.891976353363134E-9</v>
       </c>
       <c r="Q15" s="6">
         <f>Monthly_Op_LC!Q15-Monthly_Dev_LC!Q15</f>
@@ -37316,9 +37366,9 @@
         <f>Monthly_Op_LC!O16-Monthly_Dev_LC!O16</f>
         <v>0</v>
       </c>
-      <c r="P16" s="21">
+      <c r="P16" s="23">
         <f>Monthly_Op_LC!P16-Monthly_Dev_LC!P16</f>
-        <v>1.8388246202199809</v>
+        <v>-3.0701130526722409E-10</v>
       </c>
       <c r="Q16" s="6">
         <f>Monthly_Op_LC!Q16-Monthly_Dev_LC!Q16</f>
@@ -37501,9 +37551,9 @@
         <f>Monthly_Op_LC!O17-Monthly_Dev_LC!O17</f>
         <v>0</v>
       </c>
-      <c r="P17" s="21">
+      <c r="P17" s="23">
         <f>Monthly_Op_LC!P17-Monthly_Dev_LC!P17</f>
-        <v>1.3430510698269984</v>
+        <v>1.6160015547939111E-9</v>
       </c>
       <c r="Q17" s="6">
         <f>Monthly_Op_LC!Q17-Monthly_Dev_LC!Q17</f>
@@ -37686,9 +37736,9 @@
         <f>Monthly_Op_LC!O18-Monthly_Dev_LC!O18</f>
         <v>0</v>
       </c>
-      <c r="P18" s="21">
+      <c r="P18" s="23">
         <f>Monthly_Op_LC!P18-Monthly_Dev_LC!P18</f>
-        <v>1.8401277164059877</v>
+        <v>-4.0017766878008842E-11</v>
       </c>
       <c r="Q18" s="6">
         <f>Monthly_Op_LC!Q18-Monthly_Dev_LC!Q18</f>
@@ -37871,9 +37921,9 @@
         <f>Monthly_Op_LC!O19-Monthly_Dev_LC!O19</f>
         <v>0</v>
       </c>
-      <c r="P19" s="21">
+      <c r="P19" s="23">
         <f>Monthly_Op_LC!P19-Monthly_Dev_LC!P19</f>
-        <v>1.7866293958429935</v>
+        <v>-2.6760176297102589E-9</v>
       </c>
       <c r="Q19" s="6">
         <f>Monthly_Op_LC!Q19-Monthly_Dev_LC!Q19</f>
@@ -38056,9 +38106,9 @@
         <f>Monthly_Op_LC!O20-Monthly_Dev_LC!O20</f>
         <v>0</v>
       </c>
-      <c r="P20" s="21">
+      <c r="P20" s="23">
         <f>Monthly_Op_LC!P20-Monthly_Dev_LC!P20</f>
-        <v>1.4719527240349919</v>
+        <v>4.1097791836364195E-10</v>
       </c>
       <c r="Q20" s="6">
         <f>Monthly_Op_LC!Q20-Monthly_Dev_LC!Q20</f>
@@ -38241,9 +38291,9 @@
         <f>Monthly_Op_LC!O21-Monthly_Dev_LC!O21</f>
         <v>0</v>
       </c>
-      <c r="P21" s="21">
+      <c r="P21" s="23">
         <f>Monthly_Op_LC!P21-Monthly_Dev_LC!P21</f>
-        <v>1.1166002693009887</v>
+        <v>-1.8985701899509877E-11</v>
       </c>
       <c r="Q21" s="6">
         <f>Monthly_Op_LC!Q21-Monthly_Dev_LC!Q21</f>
@@ -38426,9 +38476,9 @@
         <f>Monthly_Op_LC!O22-Monthly_Dev_LC!O22</f>
         <v>0</v>
       </c>
-      <c r="P22" s="21">
+      <c r="P22" s="23">
         <f>Monthly_Op_LC!P22-Monthly_Dev_LC!P22</f>
-        <v>0.95268846597798529</v>
+        <v>4.1377006709808484E-8</v>
       </c>
       <c r="Q22" s="6">
         <f>Monthly_Op_LC!Q22-Monthly_Dev_LC!Q22</f>
@@ -38611,9 +38661,9 @@
         <f>Monthly_Op_LC!O23-Monthly_Dev_LC!O23</f>
         <v>0</v>
       </c>
-      <c r="P23" s="21">
+      <c r="P23" s="23">
         <f>Monthly_Op_LC!P23-Monthly_Dev_LC!P23</f>
-        <v>1.3489139532040326</v>
+        <v>2.0290258362365421E-9</v>
       </c>
       <c r="Q23" s="6">
         <f>Monthly_Op_LC!Q23-Monthly_Dev_LC!Q23</f>
@@ -38796,9 +38846,9 @@
         <f>Monthly_Op_LC!O24-Monthly_Dev_LC!O24</f>
         <v>0</v>
       </c>
-      <c r="P24" s="21">
+      <c r="P24" s="23">
         <f>Monthly_Op_LC!P24-Monthly_Dev_LC!P24</f>
-        <v>1.4167894276870356</v>
+        <v>-2.7189003048988525E-8</v>
       </c>
       <c r="Q24" s="6">
         <f>Monthly_Op_LC!Q24-Monthly_Dev_LC!Q24</f>
@@ -38981,9 +39031,9 @@
         <f>Monthly_Op_LC!O25-Monthly_Dev_LC!O25</f>
         <v>0</v>
       </c>
-      <c r="P25" s="21">
+      <c r="P25" s="23">
         <f>Monthly_Op_LC!P25-Monthly_Dev_LC!P25</f>
-        <v>1.5973763884549612</v>
+        <v>2.0078971374459798E-8</v>
       </c>
       <c r="Q25" s="6">
         <f>Monthly_Op_LC!Q25-Monthly_Dev_LC!Q25</f>
@@ -39166,9 +39216,9 @@
         <f>Monthly_Op_LC!O26-Monthly_Dev_LC!O26</f>
         <v>0</v>
       </c>
-      <c r="P26" s="21">
+      <c r="P26" s="23">
         <f>Monthly_Op_LC!P26-Monthly_Dev_LC!P26</f>
-        <v>1.638450512969996</v>
+        <v>5.0198423195979558E-10</v>
       </c>
       <c r="Q26" s="6">
         <f>Monthly_Op_LC!Q26-Monthly_Dev_LC!Q26</f>
@@ -39351,9 +39401,9 @@
         <f>Monthly_Op_LC!O27-Monthly_Dev_LC!O27</f>
         <v>0</v>
       </c>
-      <c r="P27" s="21">
+      <c r="P27" s="23">
         <f>Monthly_Op_LC!P27-Monthly_Dev_LC!P27</f>
-        <v>1.6322120850120427</v>
+        <v>1.261014404008165E-9</v>
       </c>
       <c r="Q27" s="6">
         <f>Monthly_Op_LC!Q27-Monthly_Dev_LC!Q27</f>
@@ -39495,7 +39545,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
-      <c r="P28" s="21"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
@@ -39567,7 +39617,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
-      <c r="P29" s="21"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
@@ -39638,7 +39688,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
-      <c r="P30" s="21"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
@@ -39695,37 +39745,37 @@
     <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="22"/>
+      <c r="P31" s="24"/>
       <c r="Q31" s="15"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
-      <c r="P32" s="22"/>
+      <c r="P32" s="24"/>
       <c r="Q32" s="15"/>
     </row>
     <row r="33" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-      <c r="P33" s="22"/>
+      <c r="P33" s="24"/>
       <c r="Q33" s="15"/>
     </row>
     <row r="34" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
-      <c r="P34" s="22"/>
+      <c r="P34" s="24"/>
       <c r="Q34" s="15"/>
     </row>
     <row r="35" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
-      <c r="P35" s="22"/>
+      <c r="P35" s="24"/>
       <c r="Q35" s="15"/>
     </row>
     <row r="36" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
-      <c r="P36" s="22"/>
+      <c r="P36" s="24"/>
       <c r="Q36" s="15"/>
     </row>
   </sheetData>

</xml_diff>